<commit_message>
Added New Unpivot Table 1
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AnnieHo\Documents\UiPath\RIBA\RIBA_ExtData_Bot11 - Copy\RIBA_ExtData_Bot11\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006E809C-80A6-4720-8032-66B9C0D117C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BC31E2-44C6-4D97-B34C-2047301BB103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -415,7 +415,7 @@
     <t>https://www.gov.uk/government/collections/building-materials-and-components-monthly-statistics-2012</t>
   </si>
   <si>
-    <t>Yes</t>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -1469,7 +1469,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4205,12 +4205,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000B998ED49CE0C34F86A981541B881BA3" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3a05d10235d6a9fd492a3a9f631ee844">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="400c0980-ee57-4191-8770-918013856bd1" xmlns:ns3="7cf5f4c0-194a-4605-9e86-e202666b6f5b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="454317dca7fdc43428dfa4fec480758a" ns2:_="" ns3:_="">
     <xsd:import namespace="400c0980-ee57-4191-8770-918013856bd1"/>
@@ -4413,6 +4407,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8632990D-292F-4A26-A371-2A34786ECA00}">
   <ds:schemaRefs>
@@ -4422,15 +4422,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC7CFB23-E6B1-4278-842C-289413FA25B9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27CACA51-C7CC-4D9C-9197-7AF79A9D0AF1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4447,4 +4438,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC7CFB23-E6B1-4278-842C-289413FA25B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>